<commit_message>
rapport et planning v1
</commit_message>
<xml_diff>
--- a/Planning_projet_version1.xlsx
+++ b/Planning_projet_version1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7a74f9203105df1/Bureau/Polytech/PeiP2/Arduino/Projet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7a74f9203105df1/Bureau/Polytech/PeiP2/Arduino/Projet/Projet_arduino/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="67" documentId="8_{E7C4B495-35DE-47D9-84AD-46F3C66C5353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EA8A043-0877-4D3B-BAE2-0682FBB67D52}"/>
@@ -184,9 +184,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -224,7 +224,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -330,7 +330,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -472,7 +472,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>